<commit_message>
update entries and change contribution to google forms
</commit_message>
<xml_diff>
--- a/cadd_vault_data.xlsx
+++ b/cadd_vault_data.xlsx
@@ -1179,7 +1179,7 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>2958</v>
+        <v>2959</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
@@ -2595,7 +2595,7 @@
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="n">
-        <v>4156</v>
+        <v>4157</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
@@ -2699,7 +2699,7 @@
       </c>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="P41" t="inlineStr">
         <is>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -3657,7 +3657,7 @@
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -3769,7 +3769,7 @@
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>15 months ago</t>
+          <t>16 months ago</t>
         </is>
       </c>
       <c r="N63" t="inlineStr"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>30 months ago</t>
+          <t>31 months ago</t>
         </is>
       </c>
       <c r="N64" t="inlineStr"/>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       <c r="O65" t="inlineStr"/>
       <c r="P65" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -4043,7 +4043,7 @@
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -4091,7 +4091,7 @@
       <c r="O67" t="inlineStr"/>
       <c r="P67" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -4131,7 +4131,7 @@
         </is>
       </c>
       <c r="K68" t="n">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="L68" t="inlineStr">
         <is>
@@ -4147,7 +4147,7 @@
       <c r="O68" t="inlineStr"/>
       <c r="P68" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>70 months ago</t>
+          <t>71 months ago</t>
         </is>
       </c>
       <c r="N74" t="inlineStr"/>
@@ -4805,7 +4805,7 @@
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="n">
-        <v>2924</v>
+        <v>2925</v>
       </c>
       <c r="P81" t="inlineStr">
         <is>
@@ -4901,7 +4901,7 @@
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="n">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="P83" t="inlineStr">
         <is>
@@ -5093,7 +5093,7 @@
       <c r="M87" t="inlineStr"/>
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="n">
-        <v>1000</v>
+        <v>1004</v>
       </c>
       <c r="P87" t="inlineStr">
         <is>
@@ -5714,7 +5714,7 @@
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>15 months ago</t>
+          <t>16 months ago</t>
         </is>
       </c>
       <c r="N100" t="inlineStr"/>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>2 months ago</t>
+          <t>3 months ago</t>
         </is>
       </c>
       <c r="N117" t="inlineStr"/>
@@ -6971,7 +6971,7 @@
       <c r="M126" t="inlineStr"/>
       <c r="N126" t="inlineStr"/>
       <c r="O126" t="n">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P126" t="inlineStr">
         <is>
@@ -7437,7 +7437,7 @@
       <c r="M136" t="inlineStr"/>
       <c r="N136" t="inlineStr"/>
       <c r="O136" t="n">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P136" t="inlineStr">
         <is>
@@ -7807,7 +7807,7 @@
       <c r="M144" t="inlineStr"/>
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="n">
-        <v>29404</v>
+        <v>29407</v>
       </c>
       <c r="P144" t="inlineStr">
         <is>
@@ -7947,7 +7947,7 @@
         </is>
       </c>
       <c r="K147" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L147" t="inlineStr">
         <is>
@@ -8711,7 +8711,7 @@
         </is>
       </c>
       <c r="K162" t="n">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="L162" t="inlineStr">
         <is>
@@ -8840,7 +8840,7 @@
       </c>
       <c r="M164" t="inlineStr">
         <is>
-          <t>23 months ago</t>
+          <t>24 months ago</t>
         </is>
       </c>
       <c r="N164" t="inlineStr"/>
@@ -9005,7 +9005,7 @@
         </is>
       </c>
       <c r="K167" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L167" t="inlineStr">
         <is>
@@ -9233,7 +9233,7 @@
         </is>
       </c>
       <c r="K171" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L171" t="inlineStr">
         <is>
@@ -9505,7 +9505,7 @@
         </is>
       </c>
       <c r="K176" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L176" t="inlineStr">
         <is>
@@ -9561,7 +9561,7 @@
         </is>
       </c>
       <c r="K177" t="n">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="L177" t="inlineStr">
         <is>
@@ -9860,7 +9860,7 @@
       </c>
       <c r="M182" t="inlineStr">
         <is>
-          <t>19 months ago</t>
+          <t>20 months ago</t>
         </is>
       </c>
       <c r="N182" t="inlineStr"/>
@@ -9909,7 +9909,7 @@
         </is>
       </c>
       <c r="K183" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L183" t="inlineStr">
         <is>
@@ -10429,7 +10429,7 @@
         </is>
       </c>
       <c r="K192" t="n">
-        <v>33780</v>
+        <v>33787</v>
       </c>
       <c r="L192" t="inlineStr">
         <is>
@@ -10604,7 +10604,7 @@
       </c>
       <c r="M195" t="inlineStr">
         <is>
-          <t>27 months ago</t>
+          <t>28 months ago</t>
         </is>
       </c>
       <c r="N195" t="inlineStr"/>
@@ -10873,7 +10873,7 @@
       <c r="I200" t="inlineStr"/>
       <c r="J200" t="inlineStr"/>
       <c r="K200" t="n">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L200" t="inlineStr">
         <is>
@@ -11273,7 +11273,7 @@
         </is>
       </c>
       <c r="K207" t="n">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L207" t="inlineStr">
         <is>
@@ -11340,7 +11340,7 @@
       </c>
       <c r="M208" t="inlineStr">
         <is>
-          <t>17 months ago</t>
+          <t>18 months ago</t>
         </is>
       </c>
       <c r="N208" t="inlineStr"/>
@@ -11566,7 +11566,7 @@
       </c>
       <c r="M212" t="inlineStr">
         <is>
-          <t>0 months ago</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="N212" t="inlineStr"/>
@@ -12513,7 +12513,7 @@
       </c>
       <c r="L229" t="inlineStr">
         <is>
-          <t>08/2024</t>
+          <t>09/2024</t>
         </is>
       </c>
       <c r="M229" t="inlineStr">
@@ -13813,7 +13813,7 @@
       <c r="M254" t="inlineStr"/>
       <c r="N254" t="inlineStr"/>
       <c r="O254" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P254" t="inlineStr">
         <is>
@@ -14828,7 +14828,7 @@
       </c>
       <c r="M275" t="inlineStr">
         <is>
-          <t>22 months ago</t>
+          <t>23 months ago</t>
         </is>
       </c>
       <c r="N275" t="inlineStr"/>
@@ -14877,7 +14877,7 @@
         </is>
       </c>
       <c r="K276" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L276" t="inlineStr">
         <is>
@@ -15377,7 +15377,7 @@
       <c r="I285" t="inlineStr"/>
       <c r="J285" t="inlineStr"/>
       <c r="K285" t="n">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L285" t="inlineStr">
         <is>
@@ -15818,7 +15818,7 @@
       </c>
       <c r="M292" t="inlineStr">
         <is>
-          <t>30 months ago</t>
+          <t>31 months ago</t>
         </is>
       </c>
       <c r="N292" t="inlineStr"/>
@@ -16253,7 +16253,7 @@
       </c>
       <c r="N299" t="inlineStr"/>
       <c r="O299" t="n">
-        <v>7371</v>
+        <v>7374</v>
       </c>
       <c r="P299" t="inlineStr">
         <is>
@@ -16479,7 +16479,7 @@
       <c r="I303" t="inlineStr"/>
       <c r="J303" t="inlineStr"/>
       <c r="K303" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L303" t="inlineStr">
         <is>
@@ -16717,7 +16717,7 @@
         </is>
       </c>
       <c r="K307" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L307" t="inlineStr">
         <is>
@@ -16899,7 +16899,7 @@
         </is>
       </c>
       <c r="K310" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L310" t="inlineStr">
         <is>
@@ -17924,7 +17924,7 @@
       </c>
       <c r="M329" t="inlineStr">
         <is>
-          <t>5 months ago</t>
+          <t>6 months ago</t>
         </is>
       </c>
       <c r="N329" t="inlineStr"/>
@@ -17976,7 +17976,7 @@
       </c>
       <c r="M330" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>2 months ago</t>
         </is>
       </c>
       <c r="N330" t="inlineStr"/>
@@ -18385,7 +18385,7 @@
       <c r="I338" t="inlineStr"/>
       <c r="J338" t="inlineStr"/>
       <c r="K338" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L338" t="inlineStr">
         <is>
@@ -19349,7 +19349,7 @@
       <c r="I356" t="inlineStr"/>
       <c r="J356" t="inlineStr"/>
       <c r="K356" t="n">
-        <v>2585</v>
+        <v>2586</v>
       </c>
       <c r="L356" t="inlineStr">
         <is>
@@ -19407,7 +19407,7 @@
         </is>
       </c>
       <c r="K357" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L357" t="inlineStr">
         <is>
@@ -21639,7 +21639,7 @@
         </is>
       </c>
       <c r="K397" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L397" t="inlineStr">
         <is>
@@ -21865,7 +21865,7 @@
       </c>
       <c r="N401" t="inlineStr"/>
       <c r="O401" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="P401" t="inlineStr">
         <is>
@@ -22954,7 +22954,7 @@
       </c>
       <c r="M423" t="inlineStr">
         <is>
-          <t>5 months ago</t>
+          <t>6 months ago</t>
         </is>
       </c>
       <c r="N423" t="inlineStr"/>
@@ -23367,7 +23367,7 @@
       <c r="M433" t="inlineStr"/>
       <c r="N433" t="inlineStr"/>
       <c r="O433" t="n">
-        <v>22287</v>
+        <v>22298</v>
       </c>
       <c r="P433" t="inlineStr">
         <is>
@@ -24061,7 +24061,7 @@
       <c r="O450" t="inlineStr"/>
       <c r="P450" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24127,7 +24127,7 @@
       </c>
       <c r="P451" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24185,7 +24185,7 @@
       </c>
       <c r="P452" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24243,7 +24243,7 @@
       </c>
       <c r="P453" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24293,11 +24293,11 @@
       </c>
       <c r="N454" t="inlineStr"/>
       <c r="O454" t="n">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="P454" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24349,7 +24349,7 @@
       <c r="O455" t="inlineStr"/>
       <c r="P455" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24403,7 +24403,7 @@
       </c>
       <c r="P456" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24455,7 +24455,7 @@
       <c r="O457" t="inlineStr"/>
       <c r="P457" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24491,7 +24491,7 @@
       <c r="I458" t="inlineStr"/>
       <c r="J458" t="inlineStr"/>
       <c r="K458" t="n">
-        <v>1687</v>
+        <v>1689</v>
       </c>
       <c r="L458" t="inlineStr">
         <is>
@@ -24509,7 +24509,7 @@
       </c>
       <c r="P458" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24545,7 +24545,7 @@
       <c r="I459" t="inlineStr"/>
       <c r="J459" t="inlineStr"/>
       <c r="K459" t="n">
-        <v>5387</v>
+        <v>5389</v>
       </c>
       <c r="L459" t="inlineStr">
         <is>
@@ -24561,7 +24561,7 @@
       <c r="O459" t="inlineStr"/>
       <c r="P459" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24619,7 +24619,7 @@
       </c>
       <c r="P460" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24673,7 +24673,7 @@
       </c>
       <c r="P461" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24727,7 +24727,7 @@
       </c>
       <c r="P462" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24781,7 +24781,7 @@
       </c>
       <c r="P463" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24833,7 +24833,7 @@
       <c r="O464" t="inlineStr"/>
       <c r="P464" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24875,7 +24875,7 @@
       <c r="O465" t="inlineStr"/>
       <c r="P465" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24923,7 +24923,7 @@
       <c r="O466" t="inlineStr"/>
       <c r="P466" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -24959,7 +24959,7 @@
       <c r="I467" t="inlineStr"/>
       <c r="J467" t="inlineStr"/>
       <c r="K467" t="n">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="L467" t="inlineStr">
         <is>
@@ -24977,7 +24977,7 @@
       </c>
       <c r="P467" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -25015,7 +25015,7 @@
       <c r="O468" t="inlineStr"/>
       <c r="P468" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -25071,7 +25071,7 @@
       <c r="O469" t="inlineStr"/>
       <c r="P469" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -25107,7 +25107,7 @@
       <c r="I470" t="inlineStr"/>
       <c r="J470" t="inlineStr"/>
       <c r="K470" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L470" t="inlineStr">
         <is>
@@ -25125,7 +25125,7 @@
       </c>
       <c r="P470" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -25178,7 +25178,7 @@
       </c>
       <c r="M471" t="inlineStr">
         <is>
-          <t>13 months ago</t>
+          <t>14 months ago</t>
         </is>
       </c>
       <c r="N471" t="inlineStr"/>
@@ -25187,7 +25187,7 @@
       </c>
       <c r="P471" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -25241,7 +25241,7 @@
       </c>
       <c r="P472" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -26105,7 +26105,7 @@
       <c r="I490" t="inlineStr"/>
       <c r="J490" t="inlineStr"/>
       <c r="K490" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="L490" t="inlineStr">
         <is>
@@ -26403,7 +26403,7 @@
         </is>
       </c>
       <c r="K495" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L495" t="inlineStr">
         <is>
@@ -27079,7 +27079,7 @@
         </is>
       </c>
       <c r="K507" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="L507" t="inlineStr">
         <is>
@@ -27145,7 +27145,7 @@
       <c r="M508" t="inlineStr"/>
       <c r="N508" t="inlineStr"/>
       <c r="O508" t="n">
-        <v>6258</v>
+        <v>6261</v>
       </c>
       <c r="P508" t="inlineStr">
         <is>
@@ -27547,7 +27547,7 @@
       </c>
       <c r="N515" t="inlineStr"/>
       <c r="O515" t="n">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="P515" t="inlineStr">
         <is>
@@ -27796,7 +27796,7 @@
       </c>
       <c r="M520" t="inlineStr">
         <is>
-          <t>2 months ago</t>
+          <t>3 months ago</t>
         </is>
       </c>
       <c r="N520" t="inlineStr"/>
@@ -27993,7 +27993,7 @@
       <c r="M524" t="inlineStr"/>
       <c r="N524" t="inlineStr"/>
       <c r="O524" t="n">
-        <v>4429</v>
+        <v>4431</v>
       </c>
       <c r="P524" t="inlineStr">
         <is>
@@ -29100,7 +29100,7 @@
       </c>
       <c r="M545" t="inlineStr">
         <is>
-          <t>4 months ago</t>
+          <t>5 months ago</t>
         </is>
       </c>
       <c r="N545" t="inlineStr"/>
@@ -29579,7 +29579,7 @@
       </c>
       <c r="N554" t="inlineStr"/>
       <c r="O554" t="n">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="P554" t="inlineStr">
         <is>
@@ -29966,7 +29966,7 @@
       </c>
       <c r="M561" t="inlineStr">
         <is>
-          <t>5 months ago</t>
+          <t>6 months ago</t>
         </is>
       </c>
       <c r="N561" t="inlineStr"/>
@@ -30033,7 +30033,7 @@
       </c>
       <c r="N562" t="inlineStr"/>
       <c r="O562" t="n">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="P562" t="inlineStr">
         <is>
@@ -30081,7 +30081,7 @@
         </is>
       </c>
       <c r="K563" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L563" t="inlineStr">
         <is>
@@ -30430,7 +30430,7 @@
       </c>
       <c r="M569" t="inlineStr">
         <is>
-          <t>36 months ago</t>
+          <t>37 months ago</t>
         </is>
       </c>
       <c r="N569" t="inlineStr"/>
@@ -30483,7 +30483,7 @@
         </is>
       </c>
       <c r="K570" t="n">
-        <v>2585</v>
+        <v>2586</v>
       </c>
       <c r="L570" t="inlineStr">
         <is>
@@ -30497,7 +30497,7 @@
       </c>
       <c r="N570" t="inlineStr"/>
       <c r="O570" t="n">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="P570" t="inlineStr">
         <is>
@@ -30911,7 +30911,7 @@
         </is>
       </c>
       <c r="K578" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L578" t="inlineStr">
         <is>
@@ -31317,7 +31317,7 @@
       </c>
       <c r="N585" t="inlineStr"/>
       <c r="O585" t="n">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="P585" t="inlineStr">
         <is>
@@ -31553,7 +31553,7 @@
       <c r="O589" t="inlineStr"/>
       <c r="P589" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -31613,7 +31613,7 @@
       <c r="O590" t="inlineStr"/>
       <c r="P590" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -31661,7 +31661,7 @@
         </is>
       </c>
       <c r="K591" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L591" t="inlineStr">
         <is>
@@ -31679,7 +31679,7 @@
       </c>
       <c r="P591" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -31743,7 +31743,7 @@
       <c r="O592" t="inlineStr"/>
       <c r="P592" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -31889,7 +31889,7 @@
       <c r="I595" t="inlineStr"/>
       <c r="J595" t="inlineStr"/>
       <c r="K595" t="n">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="L595" t="inlineStr">
         <is>
@@ -32452,7 +32452,7 @@
       </c>
       <c r="M605" t="inlineStr">
         <is>
-          <t>4 months ago</t>
+          <t>5 months ago</t>
         </is>
       </c>
       <c r="N605" t="inlineStr"/>
@@ -32956,7 +32956,7 @@
       </c>
       <c r="M615" t="inlineStr">
         <is>
-          <t>12 months ago</t>
+          <t>13 months ago</t>
         </is>
       </c>
       <c r="N615" t="inlineStr"/>
@@ -33003,7 +33003,7 @@
         </is>
       </c>
       <c r="K616" t="n">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="L616" t="inlineStr">
         <is>
@@ -33012,7 +33012,7 @@
       </c>
       <c r="M616" t="inlineStr">
         <is>
-          <t>2 months ago</t>
+          <t>3 months ago</t>
         </is>
       </c>
       <c r="N616" t="inlineStr"/>
@@ -33944,7 +33944,7 @@
       </c>
       <c r="M632" t="inlineStr">
         <is>
-          <t>29 months ago</t>
+          <t>30 months ago</t>
         </is>
       </c>
       <c r="N632" t="inlineStr"/>
@@ -34006,7 +34006,7 @@
       </c>
       <c r="M633" t="inlineStr">
         <is>
-          <t>9 months ago</t>
+          <t>10 months ago</t>
         </is>
       </c>
       <c r="N633" t="inlineStr"/>
@@ -34068,7 +34068,7 @@
       </c>
       <c r="M634" t="inlineStr">
         <is>
-          <t>42 months ago</t>
+          <t>43 months ago</t>
         </is>
       </c>
       <c r="N634" t="inlineStr"/>
@@ -34249,7 +34249,7 @@
       <c r="M637" t="inlineStr"/>
       <c r="N637" t="inlineStr"/>
       <c r="O637" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="P637" t="inlineStr">
         <is>
@@ -34398,7 +34398,7 @@
       </c>
       <c r="M640" t="inlineStr">
         <is>
-          <t>2 months ago</t>
+          <t>3 months ago</t>
         </is>
       </c>
       <c r="N640" t="inlineStr"/>
@@ -34695,7 +34695,7 @@
       </c>
       <c r="P646" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -34753,7 +34753,7 @@
       </c>
       <c r="P647" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -34809,7 +34809,7 @@
       <c r="O648" t="inlineStr"/>
       <c r="P648" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -34853,7 +34853,7 @@
         </is>
       </c>
       <c r="K649" t="n">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="L649" t="inlineStr">
         <is>
@@ -34862,7 +34862,7 @@
       </c>
       <c r="M649" t="inlineStr">
         <is>
-          <t>2 months ago</t>
+          <t>3 months ago</t>
         </is>
       </c>
       <c r="N649" t="inlineStr"/>
@@ -34871,7 +34871,7 @@
       </c>
       <c r="P649" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -34933,7 +34933,7 @@
       </c>
       <c r="P650" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -34995,7 +34995,7 @@
       </c>
       <c r="P651" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35051,7 +35051,7 @@
       <c r="O652" t="inlineStr"/>
       <c r="P652" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35097,7 +35097,7 @@
       <c r="O653" t="inlineStr"/>
       <c r="P653" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35150,7 +35150,7 @@
       </c>
       <c r="M654" t="inlineStr">
         <is>
-          <t>36 months ago</t>
+          <t>37 months ago</t>
         </is>
       </c>
       <c r="N654" t="inlineStr"/>
@@ -35159,7 +35159,7 @@
       </c>
       <c r="P654" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35221,7 +35221,7 @@
       </c>
       <c r="P655" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35283,7 +35283,7 @@
       </c>
       <c r="P656" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35343,7 +35343,7 @@
       <c r="O657" t="inlineStr"/>
       <c r="P657" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35403,7 +35403,7 @@
       <c r="O658" t="inlineStr"/>
       <c r="P658" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35465,7 +35465,7 @@
       </c>
       <c r="P659" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35529,7 +35529,7 @@
       <c r="O660" t="inlineStr"/>
       <c r="P660" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35585,7 +35585,7 @@
       <c r="O661" t="inlineStr"/>
       <c r="P661" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35649,7 +35649,7 @@
       <c r="O662" t="inlineStr"/>
       <c r="P662" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35709,7 +35709,7 @@
       <c r="O663" t="inlineStr"/>
       <c r="P663" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35762,7 +35762,7 @@
       </c>
       <c r="M664" t="inlineStr">
         <is>
-          <t>5 months ago</t>
+          <t>6 months ago</t>
         </is>
       </c>
       <c r="N664" t="inlineStr"/>
@@ -35771,7 +35771,7 @@
       </c>
       <c r="P664" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35833,7 +35833,7 @@
       </c>
       <c r="P665" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35889,7 +35889,7 @@
       <c r="O666" t="inlineStr"/>
       <c r="P666" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -35955,7 +35955,7 @@
       </c>
       <c r="P667" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36012,7 +36012,7 @@
       </c>
       <c r="M668" t="inlineStr">
         <is>
-          <t>5 months ago</t>
+          <t>6 months ago</t>
         </is>
       </c>
       <c r="N668" t="inlineStr"/>
@@ -36021,7 +36021,7 @@
       </c>
       <c r="P668" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36083,7 +36083,7 @@
       </c>
       <c r="P669" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36149,7 +36149,7 @@
       </c>
       <c r="P670" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36209,7 +36209,7 @@
       <c r="O671" t="inlineStr"/>
       <c r="P671" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36271,7 +36271,7 @@
       </c>
       <c r="P672" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36333,7 +36333,7 @@
       </c>
       <c r="P673" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36395,7 +36395,7 @@
       </c>
       <c r="P674" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36443,7 +36443,7 @@
         </is>
       </c>
       <c r="K675" t="n">
-        <v>2061</v>
+        <v>2063</v>
       </c>
       <c r="L675" t="inlineStr">
         <is>
@@ -36461,7 +36461,7 @@
       </c>
       <c r="P675" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36527,7 +36527,7 @@
       </c>
       <c r="P676" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36593,7 +36593,7 @@
       </c>
       <c r="P677" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36659,7 +36659,7 @@
       </c>
       <c r="P678" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36719,7 +36719,7 @@
       <c r="O679" t="inlineStr"/>
       <c r="P679" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36775,7 +36775,7 @@
       <c r="O680" t="inlineStr"/>
       <c r="P680" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36831,7 +36831,7 @@
       <c r="O681" t="inlineStr"/>
       <c r="P681" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36897,7 +36897,7 @@
       </c>
       <c r="P682" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -36959,7 +36959,7 @@
       </c>
       <c r="P683" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -37003,7 +37003,7 @@
       </c>
       <c r="P684" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -37052,7 +37052,7 @@
       </c>
       <c r="M685" t="inlineStr">
         <is>
-          <t>36 months ago</t>
+          <t>37 months ago</t>
         </is>
       </c>
       <c r="N685" t="inlineStr"/>
@@ -39163,7 +39163,7 @@
       </c>
       <c r="N723" t="inlineStr"/>
       <c r="O723" t="n">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="P723" t="inlineStr">
         <is>
@@ -41103,7 +41103,7 @@
       <c r="M758" t="inlineStr"/>
       <c r="N758" t="inlineStr"/>
       <c r="O758" t="n">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="P758" t="inlineStr">
         <is>
@@ -42089,7 +42089,7 @@
         </is>
       </c>
       <c r="K775" t="n">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="L775" t="inlineStr">
         <is>
@@ -42859,7 +42859,7 @@
       <c r="M788" t="inlineStr"/>
       <c r="N788" t="inlineStr"/>
       <c r="O788" t="n">
-        <v>29404</v>
+        <v>29407</v>
       </c>
       <c r="P788" t="inlineStr">
         <is>
@@ -43113,7 +43113,7 @@
       <c r="M793" t="inlineStr"/>
       <c r="N793" t="inlineStr"/>
       <c r="O793" t="n">
-        <v>8086</v>
+        <v>8089</v>
       </c>
       <c r="P793" t="inlineStr">
         <is>
@@ -43161,7 +43161,7 @@
       <c r="M794" t="inlineStr"/>
       <c r="N794" t="inlineStr"/>
       <c r="O794" t="n">
-        <v>8882</v>
+        <v>8885</v>
       </c>
       <c r="P794" t="inlineStr">
         <is>
@@ -43321,7 +43321,7 @@
       <c r="M797" t="inlineStr"/>
       <c r="N797" t="inlineStr"/>
       <c r="O797" t="n">
-        <v>22521</v>
+        <v>22539</v>
       </c>
       <c r="P797" t="inlineStr">
         <is>
@@ -43435,7 +43435,7 @@
       </c>
       <c r="N799" t="inlineStr"/>
       <c r="O799" t="n">
-        <v>4509</v>
+        <v>4511</v>
       </c>
       <c r="P799" t="inlineStr">
         <is>
@@ -43579,7 +43579,7 @@
         </is>
       </c>
       <c r="K802" t="n">
-        <v>3106</v>
+        <v>3107</v>
       </c>
       <c r="L802" t="inlineStr">
         <is>
@@ -43693,7 +43693,7 @@
         </is>
       </c>
       <c r="K804" t="n">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="L804" t="inlineStr">
         <is>
@@ -43801,7 +43801,7 @@
         </is>
       </c>
       <c r="K806" t="n">
-        <v>2707</v>
+        <v>2710</v>
       </c>
       <c r="L806" t="inlineStr">
         <is>
@@ -43929,7 +43929,7 @@
       <c r="M808" t="inlineStr"/>
       <c r="N808" t="inlineStr"/>
       <c r="O808" t="n">
-        <v>1621</v>
+        <v>1623</v>
       </c>
       <c r="P808" t="inlineStr">
         <is>
@@ -43977,7 +43977,7 @@
         </is>
       </c>
       <c r="K809" t="n">
-        <v>1981</v>
+        <v>1983</v>
       </c>
       <c r="L809" t="inlineStr">
         <is>
@@ -43991,7 +43991,7 @@
       </c>
       <c r="N809" t="inlineStr"/>
       <c r="O809" t="n">
-        <v>3309</v>
+        <v>3311</v>
       </c>
       <c r="P809" t="inlineStr">
         <is>
@@ -44039,7 +44039,7 @@
         </is>
       </c>
       <c r="K810" t="n">
-        <v>12268</v>
+        <v>12274</v>
       </c>
       <c r="L810" t="inlineStr">
         <is>
@@ -44053,7 +44053,7 @@
       </c>
       <c r="N810" t="inlineStr"/>
       <c r="O810" t="n">
-        <v>22521</v>
+        <v>22539</v>
       </c>
       <c r="P810" t="inlineStr">
         <is>
@@ -44269,7 +44269,7 @@
       </c>
       <c r="N814" t="inlineStr"/>
       <c r="O814" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P814" t="inlineStr">
         <is>
@@ -44393,7 +44393,7 @@
       </c>
       <c r="N816" t="inlineStr"/>
       <c r="O816" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P816" t="inlineStr">
         <is>
@@ -44656,7 +44656,7 @@
       </c>
       <c r="M821" t="inlineStr">
         <is>
-          <t>49 months ago</t>
+          <t>50 months ago</t>
         </is>
       </c>
       <c r="N821" t="inlineStr"/>
@@ -45839,7 +45839,7 @@
       <c r="M845" t="inlineStr"/>
       <c r="N845" t="inlineStr"/>
       <c r="O845" t="n">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="P845" t="inlineStr">
         <is>
@@ -46079,7 +46079,7 @@
       <c r="M850" t="inlineStr"/>
       <c r="N850" t="inlineStr"/>
       <c r="O850" t="n">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="P850" t="inlineStr">
         <is>
@@ -46319,7 +46319,7 @@
       <c r="M855" t="inlineStr"/>
       <c r="N855" t="inlineStr"/>
       <c r="O855" t="n">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="P855" t="inlineStr">
         <is>
@@ -46367,7 +46367,7 @@
       <c r="M856" t="inlineStr"/>
       <c r="N856" t="inlineStr"/>
       <c r="O856" t="n">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="P856" t="inlineStr">
         <is>
@@ -47625,7 +47625,7 @@
       </c>
       <c r="N882" t="inlineStr"/>
       <c r="O882" t="n">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="P882" t="inlineStr">
         <is>
@@ -47883,7 +47883,7 @@
       <c r="M887" t="inlineStr"/>
       <c r="N887" t="inlineStr"/>
       <c r="O887" t="n">
-        <v>2696</v>
+        <v>2697</v>
       </c>
       <c r="P887" t="inlineStr">
         <is>
@@ -48046,7 +48046,7 @@
       </c>
       <c r="M890" t="inlineStr">
         <is>
-          <t>8 months ago</t>
+          <t>9 months ago</t>
         </is>
       </c>
       <c r="N890" t="inlineStr"/>
@@ -48191,7 +48191,7 @@
       <c r="M893" t="inlineStr"/>
       <c r="N893" t="inlineStr"/>
       <c r="O893" t="n">
-        <v>8882</v>
+        <v>8885</v>
       </c>
       <c r="P893" t="inlineStr">
         <is>
@@ -48536,7 +48536,7 @@
       </c>
       <c r="M900" t="inlineStr">
         <is>
-          <t>3 months ago</t>
+          <t>4 months ago</t>
         </is>
       </c>
       <c r="N900" t="inlineStr"/>
@@ -50321,7 +50321,7 @@
         </is>
       </c>
       <c r="K943" t="n">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="L943" t="inlineStr">
         <is>
@@ -50420,7 +50420,7 @@
       </c>
       <c r="M945" t="inlineStr">
         <is>
-          <t>38 months ago</t>
+          <t>39 months ago</t>
         </is>
       </c>
       <c r="N945" t="inlineStr"/>
@@ -50895,7 +50895,7 @@
       <c r="I955" t="inlineStr"/>
       <c r="J955" t="inlineStr"/>
       <c r="K955" t="n">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="L955" t="inlineStr">
         <is>
@@ -51031,11 +51031,11 @@
       <c r="M958" t="inlineStr"/>
       <c r="N958" t="inlineStr"/>
       <c r="O958" t="n">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="P958" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51083,11 +51083,11 @@
       <c r="M959" t="inlineStr"/>
       <c r="N959" t="inlineStr"/>
       <c r="O959" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P959" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51145,11 +51145,11 @@
       </c>
       <c r="N960" t="inlineStr"/>
       <c r="O960" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P960" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51211,7 +51211,7 @@
       </c>
       <c r="P961" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51273,7 +51273,7 @@
       </c>
       <c r="P962" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51335,7 +51335,7 @@
       </c>
       <c r="P963" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51387,7 +51387,7 @@
       </c>
       <c r="P964" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51443,7 +51443,7 @@
       <c r="O965" t="inlineStr"/>
       <c r="P965" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51491,21 +51491,21 @@
       </c>
       <c r="L966" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>09/2024</t>
         </is>
       </c>
       <c r="M966" t="inlineStr">
         <is>
-          <t>4 months ago</t>
+          <t>0 months ago</t>
         </is>
       </c>
       <c r="N966" t="inlineStr"/>
       <c r="O966" t="n">
-        <v>2170</v>
+        <v>2172</v>
       </c>
       <c r="P966" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51567,7 +51567,7 @@
       </c>
       <c r="P967" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51613,7 +51613,7 @@
       <c r="O968" t="inlineStr"/>
       <c r="P968" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51653,7 +51653,7 @@
         </is>
       </c>
       <c r="K969" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L969" t="inlineStr">
         <is>
@@ -51669,7 +51669,7 @@
       <c r="O969" t="inlineStr"/>
       <c r="P969" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51725,7 +51725,7 @@
       </c>
       <c r="P970" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51781,7 +51781,7 @@
       <c r="O971" t="inlineStr"/>
       <c r="P971" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51839,7 +51839,7 @@
       </c>
       <c r="P972" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51887,7 +51887,7 @@
       </c>
       <c r="P973" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -51949,7 +51949,7 @@
       </c>
       <c r="P974" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52007,7 +52007,7 @@
       </c>
       <c r="P975" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52063,7 +52063,7 @@
       <c r="O976" t="inlineStr"/>
       <c r="P976" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52119,7 +52119,7 @@
       </c>
       <c r="P977" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52181,7 +52181,7 @@
       </c>
       <c r="P978" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52243,7 +52243,7 @@
       </c>
       <c r="P979" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52305,7 +52305,7 @@
       </c>
       <c r="P980" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52367,7 +52367,7 @@
       </c>
       <c r="P981" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52419,7 +52419,7 @@
       </c>
       <c r="P982" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52481,7 +52481,7 @@
       </c>
       <c r="P983" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52529,11 +52529,11 @@
       <c r="M984" t="inlineStr"/>
       <c r="N984" t="inlineStr"/>
       <c r="O984" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P984" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52587,11 +52587,11 @@
       </c>
       <c r="N985" t="inlineStr"/>
       <c r="O985" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P985" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52657,7 +52657,7 @@
       </c>
       <c r="P986" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52707,7 +52707,7 @@
       <c r="O987" t="inlineStr"/>
       <c r="P987" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52765,7 +52765,7 @@
       </c>
       <c r="P988" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52818,7 +52818,7 @@
       </c>
       <c r="M989" t="inlineStr">
         <is>
-          <t>2 months ago</t>
+          <t>3 months ago</t>
         </is>
       </c>
       <c r="N989" t="inlineStr"/>
@@ -52827,7 +52827,7 @@
       </c>
       <c r="P989" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52869,7 +52869,7 @@
       <c r="O990" t="inlineStr"/>
       <c r="P990" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52913,7 +52913,7 @@
       </c>
       <c r="P991" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -52965,7 +52965,7 @@
       </c>
       <c r="P992" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53027,7 +53027,7 @@
       </c>
       <c r="P993" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53085,7 +53085,7 @@
       </c>
       <c r="P994" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53147,7 +53147,7 @@
       </c>
       <c r="P995" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53209,7 +53209,7 @@
       </c>
       <c r="P996" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53271,7 +53271,7 @@
       </c>
       <c r="P997" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53327,7 +53327,7 @@
       <c r="O998" t="inlineStr"/>
       <c r="P998" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53383,7 +53383,7 @@
       <c r="O999" t="inlineStr"/>
       <c r="P999" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53435,7 +53435,7 @@
       </c>
       <c r="P1000" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53484,7 +53484,7 @@
       </c>
       <c r="M1001" t="inlineStr">
         <is>
-          <t>78 months ago</t>
+          <t>79 months ago</t>
         </is>
       </c>
       <c r="N1001" t="inlineStr"/>
@@ -53493,7 +53493,7 @@
       </c>
       <c r="P1001" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53551,7 +53551,7 @@
       </c>
       <c r="P1002" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53595,7 +53595,7 @@
       </c>
       <c r="P1003" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53639,7 +53639,7 @@
       </c>
       <c r="P1004" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53683,7 +53683,7 @@
       </c>
       <c r="P1005" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53727,7 +53727,7 @@
       </c>
       <c r="P1006" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53771,7 +53771,7 @@
       </c>
       <c r="P1007" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53820,7 +53820,7 @@
       </c>
       <c r="M1008" t="inlineStr">
         <is>
-          <t>17 months ago</t>
+          <t>18 months ago</t>
         </is>
       </c>
       <c r="N1008" t="inlineStr"/>
@@ -53829,7 +53829,7 @@
       </c>
       <c r="P1008" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53887,7 +53887,7 @@
       </c>
       <c r="P1009" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -53949,7 +53949,7 @@
       </c>
       <c r="P1010" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54011,7 +54011,7 @@
       </c>
       <c r="P1011" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54063,7 +54063,7 @@
       </c>
       <c r="P1012" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54121,7 +54121,7 @@
       </c>
       <c r="P1013" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54165,7 +54165,7 @@
         </is>
       </c>
       <c r="K1014" t="n">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="L1014" t="inlineStr">
         <is>
@@ -54181,7 +54181,7 @@
       <c r="O1014" t="inlineStr"/>
       <c r="P1014" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54237,7 +54237,7 @@
       <c r="O1015" t="inlineStr"/>
       <c r="P1015" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54297,7 +54297,7 @@
       <c r="O1016" t="inlineStr"/>
       <c r="P1016" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54359,7 +54359,7 @@
       </c>
       <c r="P1017" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54415,7 +54415,7 @@
       <c r="O1018" t="inlineStr"/>
       <c r="P1018" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54471,7 +54471,7 @@
       <c r="O1019" t="inlineStr"/>
       <c r="P1019" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54533,7 +54533,7 @@
       </c>
       <c r="P1020" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54595,7 +54595,7 @@
       </c>
       <c r="P1021" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54653,7 +54653,7 @@
       </c>
       <c r="P1022" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54715,7 +54715,7 @@
       </c>
       <c r="P1023" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54767,7 +54767,7 @@
       </c>
       <c r="P1024" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54825,7 +54825,7 @@
       </c>
       <c r="P1025" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54885,7 +54885,7 @@
       <c r="O1026" t="inlineStr"/>
       <c r="P1026" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -54947,7 +54947,7 @@
       </c>
       <c r="P1027" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55009,7 +55009,7 @@
       </c>
       <c r="P1028" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55071,7 +55071,7 @@
       </c>
       <c r="P1029" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55133,7 +55133,7 @@
       </c>
       <c r="P1030" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55195,7 +55195,7 @@
       </c>
       <c r="P1031" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55257,7 +55257,7 @@
       </c>
       <c r="P1032" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55301,7 +55301,7 @@
         </is>
       </c>
       <c r="K1033" t="n">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="L1033" t="inlineStr">
         <is>
@@ -55317,7 +55317,7 @@
       <c r="O1033" t="inlineStr"/>
       <c r="P1033" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55361,7 +55361,7 @@
       <c r="I1034" t="inlineStr"/>
       <c r="J1034" t="inlineStr"/>
       <c r="K1034" t="n">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="L1034" t="inlineStr">
         <is>
@@ -55377,7 +55377,7 @@
       <c r="O1034" t="inlineStr"/>
       <c r="P1034" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55439,7 +55439,7 @@
       </c>
       <c r="P1035" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55483,7 +55483,7 @@
         </is>
       </c>
       <c r="K1036" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L1036" t="inlineStr">
         <is>
@@ -55501,7 +55501,7 @@
       </c>
       <c r="P1036" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55554,7 +55554,7 @@
       </c>
       <c r="M1037" t="inlineStr">
         <is>
-          <t>0 months ago</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="N1037" t="inlineStr"/>
@@ -55563,7 +55563,7 @@
       </c>
       <c r="P1037" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55611,7 +55611,7 @@
       </c>
       <c r="P1038" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55669,7 +55669,7 @@
       </c>
       <c r="P1039" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55725,7 +55725,7 @@
       <c r="O1040" t="inlineStr"/>
       <c r="P1040" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55777,7 +55777,7 @@
       </c>
       <c r="P1041" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55835,7 +55835,7 @@
       </c>
       <c r="P1042" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55897,7 +55897,7 @@
       </c>
       <c r="P1043" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -55959,7 +55959,7 @@
       </c>
       <c r="P1044" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56021,7 +56021,7 @@
       </c>
       <c r="P1045" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56083,7 +56083,7 @@
       </c>
       <c r="P1046" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56127,7 +56127,7 @@
       </c>
       <c r="P1047" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56171,7 +56171,7 @@
       </c>
       <c r="P1048" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56233,7 +56233,7 @@
       </c>
       <c r="P1049" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56285,7 +56285,7 @@
       </c>
       <c r="P1050" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56341,7 +56341,7 @@
       <c r="O1051" t="inlineStr"/>
       <c r="P1051" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56393,7 +56393,7 @@
       </c>
       <c r="P1052" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56441,7 +56441,7 @@
       </c>
       <c r="P1053" t="inlineStr">
         <is>
-          <t>simple/abb-robotstudio</t>
+          <t>simple/abbrobotstudio</t>
         </is>
       </c>
     </row>
@@ -56960,7 +56960,7 @@
       </c>
       <c r="M1062" t="inlineStr">
         <is>
-          <t>8 months ago</t>
+          <t>9 months ago</t>
         </is>
       </c>
       <c r="N1062" t="inlineStr"/>
@@ -57321,7 +57321,7 @@
         </is>
       </c>
       <c r="K1068" t="n">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L1068" t="inlineStr">
         <is>
@@ -57856,7 +57856,7 @@
       </c>
       <c r="M1077" t="inlineStr">
         <is>
-          <t>22 months ago</t>
+          <t>23 months ago</t>
         </is>
       </c>
       <c r="N1077" t="inlineStr"/>
@@ -58135,7 +58135,7 @@
       </c>
       <c r="P1082" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -58179,7 +58179,7 @@
       </c>
       <c r="P1083" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -58223,7 +58223,7 @@
       </c>
       <c r="P1084" t="inlineStr">
         <is>
-          <t>simple/adobe-illustrator</t>
+          <t>simple/adobeillustrator</t>
         </is>
       </c>
     </row>
@@ -58309,7 +58309,7 @@
       <c r="M1086" t="inlineStr"/>
       <c r="N1086" t="inlineStr"/>
       <c r="O1086" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P1086" t="inlineStr">
         <is>
@@ -59362,7 +59362,7 @@
       </c>
       <c r="M1105" t="inlineStr">
         <is>
-          <t>3 months ago</t>
+          <t>4 months ago</t>
         </is>
       </c>
       <c r="N1105" t="inlineStr"/>
@@ -59836,7 +59836,7 @@
       </c>
       <c r="M1113" t="inlineStr">
         <is>
-          <t>35 months ago</t>
+          <t>36 months ago</t>
         </is>
       </c>
       <c r="N1113" t="inlineStr"/>
@@ -62234,7 +62234,7 @@
       </c>
       <c r="M1153" t="inlineStr">
         <is>
-          <t>16 months ago</t>
+          <t>17 months ago</t>
         </is>
       </c>
       <c r="N1153" t="inlineStr"/>
@@ -62416,7 +62416,7 @@
       </c>
       <c r="M1156" t="inlineStr">
         <is>
-          <t>11 months ago</t>
+          <t>12 months ago</t>
         </is>
       </c>
       <c r="N1156" t="inlineStr"/>
@@ -63805,7 +63805,7 @@
         </is>
       </c>
       <c r="K1180" t="n">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="L1180" t="inlineStr">
         <is>
@@ -64236,7 +64236,7 @@
       </c>
       <c r="M1188" t="inlineStr">
         <is>
-          <t>36 months ago</t>
+          <t>37 months ago</t>
         </is>
       </c>
       <c r="N1188" t="inlineStr"/>
@@ -64285,7 +64285,7 @@
         </is>
       </c>
       <c r="K1189" t="n">
-        <v>2585</v>
+        <v>2586</v>
       </c>
       <c r="L1189" t="inlineStr">
         <is>
@@ -64299,7 +64299,7 @@
       </c>
       <c r="N1189" t="inlineStr"/>
       <c r="O1189" t="n">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="P1189" t="inlineStr">
         <is>
@@ -65033,7 +65033,7 @@
         </is>
       </c>
       <c r="K1203" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L1203" t="inlineStr">
         <is>
@@ -65891,7 +65891,7 @@
       <c r="M1219" t="inlineStr"/>
       <c r="N1219" t="inlineStr"/>
       <c r="O1219" t="n">
-        <v>6466</v>
+        <v>6468</v>
       </c>
       <c r="P1219" t="inlineStr">
         <is>
@@ -65987,7 +65987,7 @@
       <c r="M1221" t="inlineStr"/>
       <c r="N1221" t="inlineStr"/>
       <c r="O1221" t="n">
-        <v>36999</v>
+        <v>37007</v>
       </c>
       <c r="P1221" t="inlineStr">
         <is>
@@ -66035,7 +66035,7 @@
       <c r="M1222" t="inlineStr"/>
       <c r="N1222" t="inlineStr"/>
       <c r="O1222" t="n">
-        <v>3811</v>
+        <v>3813</v>
       </c>
       <c r="P1222" t="inlineStr">
         <is>
@@ -66553,7 +66553,7 @@
       <c r="M1233" t="inlineStr"/>
       <c r="N1233" t="inlineStr"/>
       <c r="O1233" t="n">
-        <v>48291</v>
+        <v>48303</v>
       </c>
       <c r="P1233" t="inlineStr">
         <is>
@@ -66787,7 +66787,7 @@
       <c r="M1238" t="inlineStr"/>
       <c r="N1238" t="inlineStr"/>
       <c r="O1238" t="n">
-        <v>4271</v>
+        <v>4272</v>
       </c>
       <c r="P1238" t="inlineStr">
         <is>
@@ -67561,7 +67561,7 @@
       <c r="M1255" t="inlineStr"/>
       <c r="N1255" t="inlineStr"/>
       <c r="O1255" t="n">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="P1255" t="inlineStr">
         <is>
@@ -67945,7 +67945,7 @@
       <c r="M1263" t="inlineStr"/>
       <c r="N1263" t="inlineStr"/>
       <c r="O1263" t="n">
-        <v>5595</v>
+        <v>5597</v>
       </c>
       <c r="P1263" t="inlineStr">
         <is>
@@ -67985,7 +67985,7 @@
         </is>
       </c>
       <c r="K1264" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L1264" t="inlineStr">
         <is>
@@ -67994,7 +67994,7 @@
       </c>
       <c r="M1264" t="inlineStr">
         <is>
-          <t>4 months ago</t>
+          <t>5 months ago</t>
         </is>
       </c>
       <c r="N1264" t="inlineStr"/>
@@ -68405,7 +68405,7 @@
       <c r="M1272" t="inlineStr"/>
       <c r="N1272" t="inlineStr"/>
       <c r="O1272" t="n">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="P1272" t="inlineStr">
         <is>
@@ -68454,7 +68454,7 @@
       </c>
       <c r="M1273" t="inlineStr">
         <is>
-          <t>30 months ago</t>
+          <t>31 months ago</t>
         </is>
       </c>
       <c r="N1273" t="inlineStr"/>

</xml_diff>